<commit_message>
chore(xlsx-demo): extend sample template with dates, numbers and formula
</commit_message>
<xml_diff>
--- a/packages/xlsx/tests/fixtures/result.xlsx
+++ b/packages/xlsx/tests/fixtures/result.xlsx
@@ -4,16 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Hoja1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Nombre: Germán</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Name: Germán</t>
+  </si>
+  <si>
+    <t>Date: Mon Jan 01 2024 21:00:00 GMT-0300 (Argentina Standard Time)</t>
   </si>
   <si>
     <t>ID: 001</t>
@@ -22,10 +25,25 @@
     <t>Qty: 2</t>
   </si>
   <si>
+    <t>Price: 120.5</t>
+  </si>
+  <si>
+    <t>Item date: Tue Jan 02 2024 21:00:00 GMT-0300 (Argentina Standard Time)</t>
+  </si>
+  <si>
+    <t>Missing: [[items.missingProp]]</t>
+  </si>
+  <si>
     <t>ID: 002</t>
   </si>
   <si>
-    <t>Qty: 1</t>
+    <t>Qty: 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item date: </t>
   </si>
 </sst>
 </file>
@@ -402,28 +420,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <f>B2*C2</f>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <f>B2*C2</f>
       </c>
     </row>
   </sheetData>

</xml_diff>